<commit_message>
validation for duplicate faces done
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
@@ -534,6 +534,50 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Jayaram</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>24/11/2024</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>13:29:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Abhishek</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>24/11/2024</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>13:30:02</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>